<commit_message>
create training session psychopy and stim table xlsx
</commit_message>
<xml_diff>
--- a/AOE_final_randomized_trials.xlsx
+++ b/AOE_final_randomized_trials.xlsx
@@ -486,24 +486,24 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>robot_right_3</t>
+          <t>robot_right_4</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_3.mp4</t>
+          <t>./stimuli/robot_right_4.mp4</t>
         </is>
       </c>
       <c r="G2" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -517,12 +517,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>robot_left_2</t>
+          <t>human_right_2</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -535,11 +535,11 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_2.mp4</t>
+          <t>./stimuli/human_right_2_f.mp4</t>
         </is>
       </c>
       <c r="G3" t="n">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -553,29 +553,29 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>robot_right_4</t>
+          <t>human_left_2</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_4.mp4</t>
+          <t>./stimuli/human_left_2_m.mp4</t>
         </is>
       </c>
       <c r="G4" t="n">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -589,29 +589,29 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>human_left_4</t>
+          <t>robot_left_2</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_4_f.mp4</t>
+          <t>./stimuli/robot_left_2.mp4</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -625,29 +625,29 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>human_right_0</t>
+          <t>robot_left_1</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_0_m.mp4</t>
+          <t>./stimuli/robot_left_1.mp4</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -661,29 +661,29 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>human_right_0</t>
+          <t>human_left_4</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_0_f.mp4</t>
+          <t>./stimuli/human_left_4_m.mp4</t>
         </is>
       </c>
       <c r="G7" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -697,12 +697,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>human_right_4</t>
+          <t>human_left_4</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -715,11 +715,11 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_4_f.mp4</t>
+          <t>./stimuli/human_left_4_f.mp4</t>
         </is>
       </c>
       <c r="G8" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -733,29 +733,29 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>human_left_2</t>
+          <t>robot_right_4</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_2_m.mp4</t>
+          <t>./stimuli/robot_right_4.mp4</t>
         </is>
       </c>
       <c r="G9" t="n">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -774,24 +774,24 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>robot_left_0</t>
+          <t>robot_left_2</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_0.mp4</t>
+          <t>./stimuli/robot_left_2.mp4</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -805,29 +805,29 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>human_left_3</t>
+          <t>human_right_0</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_3_f.mp4</t>
+          <t>./stimuli/human_right_0_f.mp4</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -841,29 +841,29 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>human_right_4</t>
+          <t>human_left_3</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_4_m.mp4</t>
+          <t>./stimuli/human_left_3_m.mp4</t>
         </is>
       </c>
       <c r="G12" t="n">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -877,29 +877,29 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>robot_right_4</t>
+          <t>human_right_1</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_4.mp4</t>
+          <t>./stimuli/human_right_1_m.mp4</t>
         </is>
       </c>
       <c r="G13" t="n">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -913,29 +913,29 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>human_right_0</t>
+          <t>human_left_4</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_0_f.mp4</t>
+          <t>./stimuli/human_left_4_f.mp4</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -949,12 +949,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>robot_right_3</t>
+          <t>human_left_3</t>
         </is>
       </c>
       <c r="D15" t="n">
@@ -967,11 +967,11 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_3.mp4</t>
+          <t>./stimuli/human_left_3_m.mp4</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -985,29 +985,29 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>human_right_3</t>
+          <t>robot_left_4</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_3_f.mp4</t>
+          <t>./stimuli/robot_left_4.mp4</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1021,29 +1021,29 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>robot_right_1</t>
+          <t>human_right_0</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_1.mp4</t>
+          <t>./stimuli/human_right_0_f.mp4</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1057,29 +1057,29 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>human_left_3</t>
+          <t>robot_right_4</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_3_m.mp4</t>
+          <t>./stimuli/robot_right_4.mp4</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1098,24 +1098,24 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>human_right_4</t>
+          <t>human_right_2</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_4_f.mp4</t>
+          <t>./stimuli/human_right_2_m.mp4</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1129,29 +1129,29 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>human_right_3</t>
+          <t>robot_left_0</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_3_f.mp4</t>
+          <t>./stimuli/robot_left_0.mp4</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1165,12 +1165,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>human_right_2</t>
+          <t>human_left_2</t>
         </is>
       </c>
       <c r="D21" t="n">
@@ -1183,11 +1183,11 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_2_m.mp4</t>
+          <t>./stimuli/human_left_2_m.mp4</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1206,24 +1206,24 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>robot_left_3</t>
+          <t>robot_left_2</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_3.mp4</t>
+          <t>./stimuli/robot_left_2.mp4</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1237,12 +1237,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>robot_right_0</t>
+          <t>human_right_0</t>
         </is>
       </c>
       <c r="D23" t="n">
@@ -1255,11 +1255,11 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_0.mp4</t>
+          <t>./stimuli/human_right_0_m.mp4</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1273,29 +1273,29 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>robot_right_0</t>
+          <t>human_right_4</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_0.mp4</t>
+          <t>./stimuli/human_right_4_m.mp4</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1309,29 +1309,29 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>human_right_0</t>
+          <t>human_left_2</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_0_m.mp4</t>
+          <t>./stimuli/human_left_2_f.mp4</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -1345,29 +1345,29 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>robot_right_2</t>
+          <t>robot_left_3</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_2.mp4</t>
+          <t>./stimuli/robot_left_3.mp4</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -1381,29 +1381,29 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>robot_right_0</t>
+          <t>human_left_1</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_0.mp4</t>
+          <t>./stimuli/human_left_1_f.mp4</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1417,29 +1417,29 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>human_left_0</t>
+          <t>robot_left_3</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_0_f.mp4</t>
+          <t>./stimuli/robot_left_3.mp4</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -1489,12 +1489,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>robot_left_2</t>
+          <t>robot_right_2</t>
         </is>
       </c>
       <c r="D30" t="n">
@@ -1507,11 +1507,11 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_2.mp4</t>
+          <t>./stimuli/robot_right_2.mp4</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -1525,29 +1525,29 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>human_left_3</t>
+          <t>human_right_2</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_3_m.mp4</t>
+          <t>./stimuli/human_right_2_m.mp4</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -1566,24 +1566,24 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>robot_right_4</t>
+          <t>robot_right_2</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_4.mp4</t>
+          <t>./stimuli/robot_right_2.mp4</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -1597,12 +1597,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>robot_right_1</t>
+          <t>human_right_1</t>
         </is>
       </c>
       <c r="D33" t="n">
@@ -1615,11 +1615,11 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_1.mp4</t>
+          <t>./stimuli/human_right_1_f.mp4</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
@@ -1633,12 +1633,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>human_left_3</t>
+          <t>robot_left_3</t>
         </is>
       </c>
       <c r="D34" t="n">
@@ -1651,11 +1651,11 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_3_m.mp4</t>
+          <t>./stimuli/robot_left_3.mp4</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>13</v>
+        <v>33</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
@@ -1669,29 +1669,29 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>human_right_2</t>
+          <t>robot_left_4</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_2_f.mp4</t>
+          <t>./stimuli/robot_left_4.mp4</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
@@ -1705,29 +1705,29 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>robot_right_0</t>
+          <t>human_right_1</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_0.mp4</t>
+          <t>./stimuli/human_right_1_f.mp4</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
@@ -1741,29 +1741,29 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>human_right_3</t>
+          <t>robot_left_1</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_3_m.mp4</t>
+          <t>./stimuli/robot_left_1.mp4</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
@@ -1782,24 +1782,24 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>robot_right_4</t>
+          <t>robot_right_1</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_4.mp4</t>
+          <t>./stimuli/robot_right_1.mp4</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
@@ -1813,29 +1813,29 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>robot_left_2</t>
+          <t>human_left_1</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_2.mp4</t>
+          <t>./stimuli/human_left_1_m.mp4</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>32</v>
+        <v>11</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
@@ -1849,29 +1849,29 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>robot_left_3</t>
+          <t>human_right_4</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_3.mp4</t>
+          <t>./stimuli/human_right_4_m.mp4</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
@@ -1885,29 +1885,29 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>human_right_2</t>
+          <t>robot_right_0</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_2_m.mp4</t>
+          <t>./stimuli/robot_right_0.mp4</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
@@ -1921,29 +1921,29 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>robot_left_0</t>
+          <t>human_right_3</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_0.mp4</t>
+          <t>./stimuli/human_right_3_f.mp4</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -1957,12 +1957,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>robot_right_3</t>
+          <t>human_left_3</t>
         </is>
       </c>
       <c r="D43" t="n">
@@ -1975,11 +1975,11 @@
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_3.mp4</t>
+          <t>./stimuli/human_left_3_m.mp4</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -1993,29 +1993,29 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>robot_left_1</t>
+          <t>robot_right_4</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_1.mp4</t>
+          <t>./stimuli/robot_right_4.mp4</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -2065,29 +2065,29 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>robot_right_2</t>
+          <t>human_right_0</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_2.mp4</t>
+          <t>./stimuli/human_right_0_f.mp4</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>42</v>
+        <v>20</v>
       </c>
       <c r="H46" t="inlineStr">
         <is>
@@ -2101,29 +2101,29 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>robot_left_4</t>
+          <t>human_right_1</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_4.mp4</t>
+          <t>./stimuli/human_right_1_m.mp4</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="H47" t="inlineStr">
         <is>
@@ -2142,24 +2142,24 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>human_left_4</t>
+          <t>human_left_0</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_4_m.mp4</t>
+          <t>./stimuli/human_left_0_m.mp4</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H48" t="inlineStr">
         <is>
@@ -2173,29 +2173,29 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>robot_right_1</t>
+          <t>robot_left_4</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_1.mp4</t>
+          <t>./stimuli/robot_left_4.mp4</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H49" t="inlineStr">
         <is>
@@ -2209,29 +2209,29 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>robot_left_3</t>
+          <t>human_right_2</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_3.mp4</t>
+          <t>./stimuli/human_right_2_f.mp4</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
@@ -2245,29 +2245,29 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>human_right_3</t>
+          <t>robot_left_1</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_3_m.mp4</t>
+          <t>./stimuli/robot_left_1.mp4</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -2317,29 +2317,29 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>human_left_0</t>
+          <t>robot_right_3</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_0_f.mp4</t>
+          <t>./stimuli/robot_right_3.mp4</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
@@ -2353,29 +2353,29 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>robot_right_2</t>
+          <t>robot_left_4</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_2.mp4</t>
+          <t>./stimuli/robot_left_4.mp4</t>
         </is>
       </c>
       <c r="G54" t="n">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
@@ -2389,29 +2389,29 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>robot_right_3</t>
+          <t>robot_left_1</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_3.mp4</t>
+          <t>./stimuli/robot_left_1.mp4</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
@@ -2430,24 +2430,24 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>robot_right_1</t>
+          <t>robot_right_0</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_1.mp4</t>
+          <t>./stimuli/robot_right_0.mp4</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
@@ -2466,24 +2466,24 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>robot_left_2</t>
+          <t>robot_left_3</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_2.mp4</t>
+          <t>./stimuli/robot_left_3.mp4</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
@@ -2497,12 +2497,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>robot_left_3</t>
+          <t>human_right_3</t>
         </is>
       </c>
       <c r="D58" t="n">
@@ -2515,11 +2515,11 @@
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_3.mp4</t>
+          <t>./stimuli/human_right_3_f.mp4</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="H58" t="inlineStr">
         <is>
@@ -2533,29 +2533,29 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>human_right_0</t>
+          <t>robot_left_4</t>
         </is>
       </c>
       <c r="D59" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_0_m.mp4</t>
+          <t>./stimuli/robot_left_4.mp4</t>
         </is>
       </c>
       <c r="G59" t="n">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="H59" t="inlineStr">
         <is>
@@ -2569,29 +2569,29 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>human_left_0</t>
+          <t>human_right_4</t>
         </is>
       </c>
       <c r="D60" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_0_m.mp4</t>
+          <t>./stimuli/human_right_4_f.mp4</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="H60" t="inlineStr">
         <is>
@@ -2605,29 +2605,29 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>robot_right_1</t>
+          <t>robot_left_2</t>
         </is>
       </c>
       <c r="D61" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_1.mp4</t>
+          <t>./stimuli/robot_left_2.mp4</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="H61" t="inlineStr">
         <is>
@@ -2641,12 +2641,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>human_right_1</t>
+          <t>robot_left_1</t>
         </is>
       </c>
       <c r="D62" t="n">
@@ -2659,11 +2659,11 @@
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_1_m.mp4</t>
+          <t>./stimuli/robot_left_1.mp4</t>
         </is>
       </c>
       <c r="G62" t="n">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
@@ -2677,29 +2677,29 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>human_left_2</t>
+          <t>robot_left_0</t>
         </is>
       </c>
       <c r="D63" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_2_f.mp4</t>
+          <t>./stimuli/robot_left_0.mp4</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
@@ -2713,29 +2713,29 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>human_left_2</t>
+          <t>robot_left_0</t>
         </is>
       </c>
       <c r="D64" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_2_f.mp4</t>
+          <t>./stimuli/robot_left_0.mp4</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
@@ -2749,29 +2749,29 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>human_left_2</t>
+          <t>human_right_3</t>
         </is>
       </c>
       <c r="D65" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_2_f.mp4</t>
+          <t>./stimuli/human_right_3_m.mp4</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H65" t="inlineStr">
         <is>
@@ -2790,24 +2790,24 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>human_left_0</t>
+          <t>human_left_2</t>
         </is>
       </c>
       <c r="D66" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_0_f.mp4</t>
+          <t>./stimuli/human_left_2_m.mp4</t>
         </is>
       </c>
       <c r="G66" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
@@ -2821,29 +2821,29 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>human_left_4</t>
+          <t>robot_left_1</t>
         </is>
       </c>
       <c r="D67" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_4_f.mp4</t>
+          <t>./stimuli/robot_left_1.mp4</t>
         </is>
       </c>
       <c r="G67" t="n">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
@@ -2857,12 +2857,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>robot_right_4</t>
+          <t>human_right_4</t>
         </is>
       </c>
       <c r="D68" t="n">
@@ -2875,11 +2875,11 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_4.mp4</t>
+          <t>./stimuli/human_right_4_f.mp4</t>
         </is>
       </c>
       <c r="G68" t="n">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="H68" t="inlineStr">
         <is>
@@ -2893,29 +2893,29 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>human_left_1</t>
+          <t>robot_right_3</t>
         </is>
       </c>
       <c r="D69" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_1_f.mp4</t>
+          <t>./stimuli/robot_right_3.mp4</t>
         </is>
       </c>
       <c r="G69" t="n">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
@@ -2929,29 +2929,29 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>human_right_0</t>
+          <t>human_left_3</t>
         </is>
       </c>
       <c r="D70" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_0_f.mp4</t>
+          <t>./stimuli/human_left_3_f.mp4</t>
         </is>
       </c>
       <c r="G70" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
@@ -2970,24 +2970,24 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>human_left_4</t>
+          <t>human_left_0</t>
         </is>
       </c>
       <c r="D71" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_4_m.mp4</t>
+          <t>./stimuli/human_left_0_m.mp4</t>
         </is>
       </c>
       <c r="G71" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
@@ -3001,29 +3001,29 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>robot_right_2</t>
+          <t>human_left_0</t>
         </is>
       </c>
       <c r="D72" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_2.mp4</t>
+          <t>./stimuli/human_left_0_m.mp4</t>
         </is>
       </c>
       <c r="G72" t="n">
-        <v>42</v>
+        <v>10</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
@@ -3042,24 +3042,24 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>human_left_4</t>
+          <t>human_left_0</t>
         </is>
       </c>
       <c r="D73" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_4_m.mp4</t>
+          <t>./stimuli/human_left_0_f.mp4</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>
@@ -3073,29 +3073,29 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>human_right_4</t>
+          <t>robot_left_3</t>
         </is>
       </c>
       <c r="D74" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_4_m.mp4</t>
+          <t>./stimuli/robot_left_3.mp4</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="H74" t="inlineStr">
         <is>
@@ -3109,29 +3109,29 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>robot_left_2</t>
+          <t>robot_right_0</t>
         </is>
       </c>
       <c r="D75" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_2.mp4</t>
+          <t>./stimuli/robot_right_0.mp4</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H75" t="inlineStr">
         <is>
@@ -3145,12 +3145,12 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>human_right_2</t>
+          <t>human_left_2</t>
         </is>
       </c>
       <c r="D76" t="n">
@@ -3163,11 +3163,11 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_2_m.mp4</t>
+          <t>./stimuli/human_left_2_f.mp4</t>
         </is>
       </c>
       <c r="G76" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="H76" t="inlineStr">
         <is>
@@ -3181,29 +3181,29 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>human_right_2</t>
+          <t>human_left_1</t>
         </is>
       </c>
       <c r="D77" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_2_f.mp4</t>
+          <t>./stimuli/human_left_1_m.mp4</t>
         </is>
       </c>
       <c r="G77" t="n">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="H77" t="inlineStr">
         <is>
@@ -3217,29 +3217,29 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>human_left_3</t>
+          <t>robot_right_1</t>
         </is>
       </c>
       <c r="D78" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_3_f.mp4</t>
+          <t>./stimuli/robot_right_1.mp4</t>
         </is>
       </c>
       <c r="G78" t="n">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="H78" t="inlineStr">
         <is>
@@ -3253,12 +3253,12 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>human_left_1</t>
+          <t>human_right_1</t>
         </is>
       </c>
       <c r="D79" t="n">
@@ -3271,11 +3271,11 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_1_f.mp4</t>
+          <t>./stimuli/human_right_1_m.mp4</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H79" t="inlineStr">
         <is>
@@ -3289,29 +3289,29 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>human_right_3</t>
+          <t>robot_left_0</t>
         </is>
       </c>
       <c r="D80" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_3_m.mp4</t>
+          <t>./stimuli/robot_left_0.mp4</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="H80" t="inlineStr">
         <is>
@@ -3325,29 +3325,29 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>human_right_1</t>
+          <t>robot_left_3</t>
         </is>
       </c>
       <c r="D81" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_1_f.mp4</t>
+          <t>./stimuli/robot_left_3.mp4</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="H81" t="inlineStr">
         <is>
@@ -3361,29 +3361,29 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>robot_right_0</t>
+          <t>human_right_3</t>
         </is>
       </c>
       <c r="D82" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_0.mp4</t>
+          <t>./stimuli/human_right_3_m.mp4</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="H82" t="inlineStr">
         <is>
@@ -3397,12 +3397,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>human_right_4</t>
+          <t>robot_right_4</t>
         </is>
       </c>
       <c r="D83" t="n">
@@ -3415,11 +3415,11 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_4_f.mp4</t>
+          <t>./stimuli/robot_right_4.mp4</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
@@ -3433,12 +3433,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>human_right_3</t>
+          <t>robot_right_3</t>
         </is>
       </c>
       <c r="D84" t="n">
@@ -3451,11 +3451,11 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_3_f.mp4</t>
+          <t>./stimuli/robot_right_3.mp4</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
@@ -3469,29 +3469,29 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>robot_left_0</t>
+          <t>robot_right_3</t>
         </is>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_0.mp4</t>
+          <t>./stimuli/robot_right_3.mp4</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
@@ -3505,29 +3505,29 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>robot_left_3</t>
+          <t>robot_right_0</t>
         </is>
       </c>
       <c r="D86" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_3.mp4</t>
+          <t>./stimuli/robot_right_0.mp4</t>
         </is>
       </c>
       <c r="G86" t="n">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="H86" t="inlineStr">
         <is>
@@ -3541,29 +3541,29 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>robot_left_3</t>
+          <t>human_right_2</t>
         </is>
       </c>
       <c r="D87" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_3.mp4</t>
+          <t>./stimuli/human_right_2_m.mp4</t>
         </is>
       </c>
       <c r="G87" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="H87" t="inlineStr">
         <is>
@@ -3577,29 +3577,29 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>robot_left_4</t>
+          <t>human_left_3</t>
         </is>
       </c>
       <c r="D88" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_4.mp4</t>
+          <t>./stimuli/human_left_3_f.mp4</t>
         </is>
       </c>
       <c r="G88" t="n">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="H88" t="inlineStr">
         <is>
@@ -3654,24 +3654,24 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>robot_right_3</t>
+          <t>robot_right_1</t>
         </is>
       </c>
       <c r="D90" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_3.mp4</t>
+          <t>./stimuli/robot_right_1.mp4</t>
         </is>
       </c>
       <c r="G90" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H90" t="inlineStr">
         <is>
@@ -3685,29 +3685,29 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>human_left_1</t>
+          <t>robot_right_3</t>
         </is>
       </c>
       <c r="D91" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_1_m.mp4</t>
+          <t>./stimuli/robot_right_3.mp4</t>
         </is>
       </c>
       <c r="G91" t="n">
-        <v>11</v>
+        <v>43</v>
       </c>
       <c r="H91" t="inlineStr">
         <is>
@@ -3721,29 +3721,29 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>human_left_3</t>
+          <t>robot_right_2</t>
         </is>
       </c>
       <c r="D92" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_3_f.mp4</t>
+          <t>./stimuli/robot_right_2.mp4</t>
         </is>
       </c>
       <c r="G92" t="n">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="H92" t="inlineStr">
         <is>
@@ -3757,29 +3757,29 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>robot_left_4</t>
+          <t>human_left_1</t>
         </is>
       </c>
       <c r="D93" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_4.mp4</t>
+          <t>./stimuli/human_left_1_f.mp4</t>
         </is>
       </c>
       <c r="G93" t="n">
-        <v>34</v>
+        <v>11</v>
       </c>
       <c r="H93" t="inlineStr">
         <is>
@@ -3793,12 +3793,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>human_left_1</t>
+          <t>robot_right_1</t>
         </is>
       </c>
       <c r="D94" t="n">
@@ -3811,11 +3811,11 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_1_f.mp4</t>
+          <t>./stimuli/robot_right_1.mp4</t>
         </is>
       </c>
       <c r="G94" t="n">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="H94" t="inlineStr">
         <is>
@@ -3829,29 +3829,29 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>robot_left_1</t>
+          <t>human_left_0</t>
         </is>
       </c>
       <c r="D95" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_1.mp4</t>
+          <t>./stimuli/human_left_0_f.mp4</t>
         </is>
       </c>
       <c r="G95" t="n">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
@@ -3870,24 +3870,24 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>robot_right_3</t>
+          <t>robot_right_1</t>
         </is>
       </c>
       <c r="D96" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>overhead arm raise</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_3.mp4</t>
+          <t>./stimuli/robot_right_1.mp4</t>
         </is>
       </c>
       <c r="G96" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
@@ -3901,12 +3901,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>human_right_4</t>
+          <t>human_left_4</t>
         </is>
       </c>
       <c r="D97" t="n">
@@ -3919,11 +3919,11 @@
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_4_m.mp4</t>
+          <t>./stimuli/human_left_4_m.mp4</t>
         </is>
       </c>
       <c r="G97" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="H97" t="inlineStr">
         <is>
@@ -3937,29 +3937,29 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>robot_left_1</t>
+          <t>human_left_2</t>
         </is>
       </c>
       <c r="D98" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_1.mp4</t>
+          <t>./stimuli/human_left_2_f.mp4</t>
         </is>
       </c>
       <c r="G98" t="n">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="H98" t="inlineStr">
         <is>
@@ -3973,12 +3973,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>robot_left_4</t>
+          <t>human_right_4</t>
         </is>
       </c>
       <c r="D99" t="n">
@@ -3991,11 +3991,11 @@
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_4.mp4</t>
+          <t>./stimuli/human_right_4_m.mp4</t>
         </is>
       </c>
       <c r="G99" t="n">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="H99" t="inlineStr">
         <is>
@@ -4009,29 +4009,29 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>human_left_2</t>
+          <t>human_right_3</t>
         </is>
       </c>
       <c r="D100" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_2_m.mp4</t>
+          <t>./stimuli/human_right_3_m.mp4</t>
         </is>
       </c>
       <c r="G100" t="n">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="H100" t="inlineStr">
         <is>
@@ -4045,29 +4045,29 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>human_right_1</t>
+          <t>robot_right_0</t>
         </is>
       </c>
       <c r="D101" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_1_m.mp4</t>
+          <t>./stimuli/robot_right_0.mp4</t>
         </is>
       </c>
       <c r="G101" t="n">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="H101" t="inlineStr">
         <is>
@@ -4081,12 +4081,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>robot_left_0</t>
+          <t>human_right_0</t>
         </is>
       </c>
       <c r="D102" t="n">
@@ -4099,11 +4099,11 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_0.mp4</t>
+          <t>./stimuli/human_right_0_m.mp4</t>
         </is>
       </c>
       <c r="G102" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H102" t="inlineStr">
         <is>
@@ -4117,29 +4117,29 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>robot_right_0</t>
+          <t>human_left_1</t>
         </is>
       </c>
       <c r="D103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_0.mp4</t>
+          <t>./stimuli/human_left_1_m.mp4</t>
         </is>
       </c>
       <c r="G103" t="n">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="H103" t="inlineStr">
         <is>
@@ -4158,24 +4158,24 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>robot_left_0</t>
+          <t>robot_left_2</t>
         </is>
       </c>
       <c r="D104" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_0.mp4</t>
+          <t>./stimuli/robot_left_2.mp4</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
@@ -4189,29 +4189,29 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>robot_left_1</t>
+          <t>human_left_4</t>
         </is>
       </c>
       <c r="D105" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_1.mp4</t>
+          <t>./stimuli/human_left_4_f.mp4</t>
         </is>
       </c>
       <c r="G105" t="n">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
@@ -4225,12 +4225,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>human_left_0</t>
+          <t>robot_left_0</t>
         </is>
       </c>
       <c r="D106" t="n">
@@ -4243,11 +4243,11 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_0_m.mp4</t>
+          <t>./stimuli/robot_left_0.mp4</t>
         </is>
       </c>
       <c r="G106" t="n">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="H106" t="inlineStr">
         <is>
@@ -4261,29 +4261,29 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>robot_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>robot_right_1</t>
+          <t>human_left_4</t>
         </is>
       </c>
       <c r="D107" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>./stimuli/robot_right_1.mp4</t>
+          <t>./stimuli/human_left_4_m.mp4</t>
         </is>
       </c>
       <c r="G107" t="n">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="H107" t="inlineStr">
         <is>
@@ -4297,29 +4297,29 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>robot_left_4</t>
+          <t>robot_right_3</t>
         </is>
       </c>
       <c r="D108" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_4.mp4</t>
+          <t>./stimuli/robot_right_3.mp4</t>
         </is>
       </c>
       <c r="G108" t="n">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H108" t="inlineStr">
         <is>
@@ -4333,29 +4333,29 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>robot_left_0</t>
+          <t>human_left_1</t>
         </is>
       </c>
       <c r="D109" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>forward-backward swing</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_0.mp4</t>
+          <t>./stimuli/human_left_1_f.mp4</t>
         </is>
       </c>
       <c r="G109" t="n">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="H109" t="inlineStr">
         <is>
@@ -4369,29 +4369,29 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>robot_left_1</t>
+          <t>human_right_0</t>
         </is>
       </c>
       <c r="D110" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_1.mp4</t>
+          <t>./stimuli/human_right_0_m.mp4</t>
         </is>
       </c>
       <c r="G110" t="n">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="H110" t="inlineStr">
         <is>
@@ -4405,29 +4405,29 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>robot_left_1</t>
+          <t>robot_right_2</t>
         </is>
       </c>
       <c r="D111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_1.mp4</t>
+          <t>./stimuli/robot_right_2.mp4</t>
         </is>
       </c>
       <c r="G111" t="n">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="H111" t="inlineStr">
         <is>
@@ -4441,12 +4441,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>human_left_4</t>
+          <t>human_right_4</t>
         </is>
       </c>
       <c r="D112" t="n">
@@ -4459,11 +4459,11 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_4_f.mp4</t>
+          <t>./stimuli/human_right_4_f.mp4</t>
         </is>
       </c>
       <c r="G112" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H112" t="inlineStr">
         <is>
@@ -4477,29 +4477,29 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>human_right_1</t>
+          <t>robot_left_2</t>
         </is>
       </c>
       <c r="D113" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>medial-lateral swing</t>
         </is>
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_1_f.mp4</t>
+          <t>./stimuli/robot_left_2.mp4</t>
         </is>
       </c>
       <c r="G113" t="n">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="H113" t="inlineStr">
         <is>
@@ -4513,29 +4513,29 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>human_right_1</t>
+          <t>robot_left_0</t>
         </is>
       </c>
       <c r="D114" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_1_f.mp4</t>
+          <t>./stimuli/robot_left_0.mp4</t>
         </is>
       </c>
       <c r="G114" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="H114" t="inlineStr">
         <is>
@@ -4549,12 +4549,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>human_left_1</t>
+          <t>human_right_1</t>
         </is>
       </c>
       <c r="D115" t="n">
@@ -4567,11 +4567,11 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_1_m.mp4</t>
+          <t>./stimuli/human_right_1_f.mp4</t>
         </is>
       </c>
       <c r="G115" t="n">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="H115" t="inlineStr">
         <is>
@@ -4585,12 +4585,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>human_left_1</t>
+          <t>robot_right_1</t>
         </is>
       </c>
       <c r="D116" t="n">
@@ -4603,11 +4603,11 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_1_m.mp4</t>
+          <t>./stimuli/robot_right_1.mp4</t>
         </is>
       </c>
       <c r="G116" t="n">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="H116" t="inlineStr">
         <is>
@@ -4621,29 +4621,29 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>robot_right</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>robot_left_4</t>
+          <t>robot_right_0</t>
         </is>
       </c>
       <c r="D117" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>waving</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_4.mp4</t>
+          <t>./stimuli/robot_right_0.mp4</t>
         </is>
       </c>
       <c r="G117" t="n">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H117" t="inlineStr">
         <is>
@@ -4662,24 +4662,24 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>human_left_2</t>
+          <t>human_left_3</t>
         </is>
       </c>
       <c r="D118" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_2_m.mp4</t>
+          <t>./stimuli/human_left_3_f.mp4</t>
         </is>
       </c>
       <c r="G118" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H118" t="inlineStr">
         <is>
@@ -4693,29 +4693,29 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>robot_left</t>
+          <t>human_right</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>robot_left_2</t>
+          <t>human_right_3</t>
         </is>
       </c>
       <c r="D119" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>medial-lateral swing</t>
+          <t>overhead arm raise</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>./stimuli/robot_left_2.mp4</t>
+          <t>./stimuli/human_right_3_f.mp4</t>
         </is>
       </c>
       <c r="G119" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="H119" t="inlineStr">
         <is>
@@ -4729,29 +4729,29 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>human_left</t>
+          <t>robot_left</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>human_left_0</t>
+          <t>robot_left_4</t>
         </is>
       </c>
       <c r="D120" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>air punching</t>
+          <t>waving</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>./stimuli/human_left_0_m.mp4</t>
+          <t>./stimuli/robot_left_4.mp4</t>
         </is>
       </c>
       <c r="G120" t="n">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="H120" t="inlineStr">
         <is>
@@ -4765,29 +4765,29 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>human_right</t>
+          <t>human_left</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>human_right_1</t>
+          <t>human_left_0</t>
         </is>
       </c>
       <c r="D121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
-          <t>forward-backward swing</t>
+          <t>air punching</t>
         </is>
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>./stimuli/human_right_1_m.mp4</t>
+          <t>./stimuli/human_left_0_f.mp4</t>
         </is>
       </c>
       <c r="G121" t="n">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="H121" t="inlineStr">
         <is>

</xml_diff>